<commit_message>
My EDA now makes sense
</commit_message>
<xml_diff>
--- a/CH-186 Column Splitting.xlsx
+++ b/CH-186 Column Splitting.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481DA596-3C44-42F6-95CE-7AD4DD1B3B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBE1298-7071-4A2E-813A-56F3F38D8E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$C$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$C$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$C$14</definedName>
   </definedNames>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="16">
   <si>
     <t>Question</t>
   </si>
@@ -787,6 +789,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="877" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{EF770F54-F5C7-40D9-9946-49BF6CDEAFB1}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K21"/>
@@ -999,7 +1028,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1158,48 +1187,322 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="str" cm="1">
-        <f t="array" ref="B12">_xlfn.REGEXEXTRACT(B3,"([aeiouAEIOU]+)|([^aeiouAEIOU]+)",1)</f>
+        <f t="array" ref="B12">_xlfn.REGEXEXTRACT(B3,"([AEIOU]+)|([^AEIOU]+)",1,1)</f>
         <v>MN12</v>
       </c>
       <c r="C12" s="7"/>
+      <c r="D12" s="5" t="str" cm="1">
+        <f t="array" ref="D12:D17">_xlfn.IFNA(_xlfn.REGEXEXTRACT(B3:B8,"[aeiou]+",0,1),"")</f>
+        <v/>
+      </c>
+      <c r="E12" t="str" cm="1">
+        <f t="array" ref="E12:E17">_xlfn.IFNA(_xlfn.REGEXEXTRACT(B3:B8,"[^aeiou]+",0,1),"")</f>
+        <v>MN12</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="str" cm="1">
-        <f t="array" ref="B13:C13">_xlfn.REGEXEXTRACT(B4,"([aeiouAEIOU]+)|([^aeiouAEIOU]+)",1)</f>
+        <f t="array" ref="B13:C13">_xlfn.REGEXEXTRACT(B4,"([AEIOU]+)|([^AEIOU]+)",1,1)</f>
         <v>AEIOU</v>
       </c>
       <c r="C13" s="7" t="str">
         <v>123</v>
       </c>
+      <c r="D13" s="5" t="str">
+        <v>AEIOU</v>
+      </c>
+      <c r="E13" t="str">
+        <v>123</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str" cm="1">
-        <f t="array" ref="B14">_xlfn.REGEXEXTRACT(B5,"([aeiouAEIOU]+)|([^aeiouAEIOU]+)",1)</f>
+        <f t="array" ref="B14">_xlfn.REGEXEXTRACT(B5,"([AEIOU]+)|([^AEIOU]+)",1,1)</f>
         <v>RS5M55</v>
       </c>
       <c r="C14" s="7"/>
+      <c r="D14" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E14" t="str">
+        <v>RS5M55</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str" cm="1">
-        <f t="array" ref="B15">_xlfn.REGEXEXTRACT(B6,"([aeiouAEIOU]+)|([^aeiouAEIOU]+)",1)</f>
+        <f t="array" ref="B15">_xlfn.REGEXEXTRACT(B6,"([AEIOU]+)|([^AEIOU]+)",1,1)</f>
         <v>FFm210</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="18" t="str">
+        <v/>
+      </c>
+      <c r="E15" t="str">
+        <v>FFm210</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str" cm="1">
-        <f t="array" ref="B16:C16">_xlfn.REGEXEXTRACT(B7,"([aeiouAEIOU]+)|([^aeiouAEIOU]+)",1)</f>
+        <f t="array" ref="B16:C16">_xlfn.REGEXEXTRACT(B7,"([AEIOU]+)|([^AEIOU]+)",1,1)</f>
         <v>OU</v>
       </c>
       <c r="C16" t="str">
         <v>LP33</v>
       </c>
+      <c r="D16" s="19" t="str">
+        <v>OU</v>
+      </c>
+      <c r="E16" t="str">
+        <v>LP33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="str" cm="1">
+        <f t="array" ref="B17">_xlfn.REGEXEXTRACT(B8,"([AEIOU]+)|([^AEIOU]+)",1,1)</f>
+        <v>aei</v>
+      </c>
+      <c r="D17" s="19" t="str">
+        <v>aei</v>
+      </c>
+      <c r="E17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="19"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69F1842-E28B-4565-8549-A5587DFCEB49}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.19921875" customWidth="1"/>
+    <col min="4" max="4" width="8.69921875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="21"/>
+      <c r="H1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="15">
+        <v>123</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="str" cm="1">
+        <f t="array" ref="B12:C17">_xlfn.LET(
+    _xlpm.rng, B3:B8,
+    _xlpm.R, _xleta.REGEXEXTRACT,
+    _xlpm.v, _xlfn.IFNA(_xlpm.R(_xlpm.rng, "[aeiou]+", , 1), ""),
+    _xlpm.cn, _xlfn.IFNA(_xlpm.R(_xlpm.rng, "[^aeiou]+", , 1), ""),
+    _xlfn.HSTACK(_xlpm.v, _xlpm.cn)
+)</f>
+        <v/>
+      </c>
+      <c r="C12" s="7" t="str">
+        <v>MN12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="str">
+        <v>AEIOU</v>
+      </c>
+      <c r="C13" s="7" t="str">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="str">
+        <v/>
+      </c>
+      <c r="C14" s="7" t="str">
+        <v>RS5M55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C15" t="str">
+        <v>FFm210</v>
+      </c>
+      <c r="D15" s="18"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="str">
+        <v>OU</v>
+      </c>
+      <c r="C16" t="str">
+        <v>LP33</v>
+      </c>
       <c r="D16" s="19"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="str" cm="1">
-        <f t="array" ref="B17">_xlfn.REGEXEXTRACT(B8,"([aeiouAEIOU]+)|([^aeiouAEIOU]+)",1)</f>
+      <c r="B17" s="4" t="str">
         <v>aei</v>
+      </c>
+      <c r="C17" t="str">
+        <v/>
       </c>
       <c r="D17" s="19"/>
     </row>

</xml_diff>